<commit_message>
fix tambahan bug -rs
</commit_message>
<xml_diff>
--- a/public/test/datatesting.xlsx
+++ b/public/test/datatesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Skripsi\webdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC5C284-8417-4918-B5AE-82BAF03C7EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74700871-B752-4FC6-9FA7-C7AC30761BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B750663C-B1F1-4950-82D1-AC2B38D2C754}"/>
   </bookViews>
@@ -5559,100 +5559,34 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DAFDCD8C-55B4-43E9-A751-09BEA25D00CE}"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="32">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -5673,34 +5607,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -5989,6 +5895,33 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -6070,6 +6003,13 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6084,41 +6024,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{727405B8-B33E-4EBA-999D-32075DC1D534}" name="Table2" displayName="Table2" ref="A1:AC501" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{727405B8-B33E-4EBA-999D-32075DC1D534}" name="Table2" displayName="Table2" ref="A1:AC501" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:AC501" xr:uid="{727405B8-B33E-4EBA-999D-32075DC1D534}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC501">
     <sortCondition ref="C1:C501"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="25" xr3:uid="{69D161F1-FF49-4491-A2B5-ACDEFB9765BB}" name="RW" dataDxfId="35"/>
-    <tableColumn id="24" xr3:uid="{426ECDE8-F452-4F84-861A-CD7DDC126AAB}" name="RT" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{928DC594-9D6F-4854-ABC8-012D2B0B6DA6}" name="NOMOR KK" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{220D8817-8C32-4889-A914-05905F1CF7C2}" name="NIK" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{2ADB0BCF-34D2-41E5-B37F-223BAF619F04}" name="NAMA LENGKAP" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{ADC4D420-0F37-4348-98E2-B4600EEAA7FB}" name="JENIS IDENTITAS" dataDxfId="9" dataCellStyle="Normal 2"/>
-    <tableColumn id="20" xr3:uid="{E498620D-2B5A-4EF9-95AF-A50FC6D40C01}" name="NIK SEMENTARA" dataDxfId="8" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{97BDEF46-18B0-4D24-A9D1-F686BB388517}" name="JENIS KELAMIN" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{3F65CB27-F410-4E83-A770-C4106F8C910D}" name="TEMPAT LAHIR" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{09E0E6C7-D5D0-4D6E-B9CF-166DCBB377B3}" name="TANGGAL LAHIR" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{581E2A00-768B-47E9-B446-DF11C60C8490}" name="AGAMA" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{B45D65E5-9F57-4251-B0CA-8DCC60BCB618}" name="PENDIDIKAN " dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{C95405B4-7425-4FDC-95D2-C9A9A0F6E404}" name="PEKERJAAN" dataDxfId="26"/>
-    <tableColumn id="27" xr3:uid="{363BA4BC-39AD-4E9E-93C4-03032BAFC915}" name="KEWARGANEGARAAN" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{743B70F3-E4F3-4172-8332-642F315B04A8}" name="STATUS PENDUDUK" dataDxfId="24"/>
-    <tableColumn id="26" xr3:uid="{9997649A-30B9-4F81-820C-F4DF24A29073}" name="STATUS DASAR" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{5177A53C-1FD9-41E0-9F46-BB71A14B5948}" name="STATUS PERKAWINAN" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{B531E2D4-1EC1-4598-9ADE-B2E6FC5DAEE0}" name="STATUS HUBUNGAN" dataDxfId="21"/>
-    <tableColumn id="29" xr3:uid="{5C4EAE11-5CDF-400A-9B24-9596D822223F}" name="NAMA AYAH" dataDxfId="20"/>
-    <tableColumn id="30" xr3:uid="{57923CE9-DC18-4B51-9372-52BE9851DDD3}" name="NAMA IBU" dataDxfId="19"/>
-    <tableColumn id="31" xr3:uid="{32DA0496-AA72-481E-BAF8-D5153E11C7A7}" name="NIK AYAH" dataDxfId="18"/>
-    <tableColumn id="32" xr3:uid="{09F32386-7DBF-41E3-90A9-33F3233D75D8}" name="NIK IBU" dataDxfId="17"/>
-    <tableColumn id="34" xr3:uid="{56F32F01-60E5-4376-A7D8-B40D44443FD6}" name="ETNIS SUKU" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{2C08E89E-E1EF-4F99-9F01-48DB11FA3130}" name="GOLONGAN DARAH" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{F89703C5-EA50-4AE5-B1D5-CC8E3059C5BA}" name="ALAMAT SEKARANG" dataDxfId="10" dataCellStyle="Normal 2"/>
-    <tableColumn id="33" xr3:uid="{CCF3BD54-E633-4ED7-B627-6D1DEAD1E311}" name="ALAMAT SEBELUMNYA" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="14" xr3:uid="{E462B6DD-29D4-4A17-AA0F-9EA81F6FD241}" name="TELEPON" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{470FBA59-E537-4ED4-BD1C-17FECE5E79A6}" name="EMAIL" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{861A2621-6363-4E65-B747-DE7EBE497051}" name="TANGGAL UPDATE DATA" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{69D161F1-FF49-4491-A2B5-ACDEFB9765BB}" name="RW" dataDxfId="28"/>
+    <tableColumn id="24" xr3:uid="{426ECDE8-F452-4F84-861A-CD7DDC126AAB}" name="RT" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{928DC594-9D6F-4854-ABC8-012D2B0B6DA6}" name="NOMOR KK" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{220D8817-8C32-4889-A914-05905F1CF7C2}" name="NIK" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{2ADB0BCF-34D2-41E5-B37F-223BAF619F04}" name="NAMA LENGKAP" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{ADC4D420-0F37-4348-98E2-B4600EEAA7FB}" name="JENIS IDENTITAS" dataDxfId="23" dataCellStyle="Normal 2"/>
+    <tableColumn id="20" xr3:uid="{E498620D-2B5A-4EF9-95AF-A50FC6D40C01}" name="NIK SEMENTARA" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{97BDEF46-18B0-4D24-A9D1-F686BB388517}" name="JENIS KELAMIN" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{3F65CB27-F410-4E83-A770-C4106F8C910D}" name="TEMPAT LAHIR" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{09E0E6C7-D5D0-4D6E-B9CF-166DCBB377B3}" name="TANGGAL LAHIR" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{581E2A00-768B-47E9-B446-DF11C60C8490}" name="AGAMA" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{B45D65E5-9F57-4251-B0CA-8DCC60BCB618}" name="PENDIDIKAN " dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{C95405B4-7425-4FDC-95D2-C9A9A0F6E404}" name="PEKERJAAN" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{363BA4BC-39AD-4E9E-93C4-03032BAFC915}" name="KEWARGANEGARAAN" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{743B70F3-E4F3-4172-8332-642F315B04A8}" name="STATUS PENDUDUK" dataDxfId="14"/>
+    <tableColumn id="26" xr3:uid="{9997649A-30B9-4F81-820C-F4DF24A29073}" name="STATUS DASAR" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{5177A53C-1FD9-41E0-9F46-BB71A14B5948}" name="STATUS PERKAWINAN" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{B531E2D4-1EC1-4598-9ADE-B2E6FC5DAEE0}" name="STATUS HUBUNGAN" dataDxfId="11"/>
+    <tableColumn id="29" xr3:uid="{5C4EAE11-5CDF-400A-9B24-9596D822223F}" name="NAMA AYAH" dataDxfId="10"/>
+    <tableColumn id="30" xr3:uid="{57923CE9-DC18-4B51-9372-52BE9851DDD3}" name="NAMA IBU" dataDxfId="9"/>
+    <tableColumn id="31" xr3:uid="{32DA0496-AA72-481E-BAF8-D5153E11C7A7}" name="NIK AYAH" dataDxfId="8"/>
+    <tableColumn id="32" xr3:uid="{09F32386-7DBF-41E3-90A9-33F3233D75D8}" name="NIK IBU" dataDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{56F32F01-60E5-4376-A7D8-B40D44443FD6}" name="ETNIS SUKU" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{2C08E89E-E1EF-4F99-9F01-48DB11FA3130}" name="GOLONGAN DARAH" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{F89703C5-EA50-4AE5-B1D5-CC8E3059C5BA}" name="ALAMAT SEKARANG" dataDxfId="4" dataCellStyle="Normal 2"/>
+    <tableColumn id="33" xr3:uid="{CCF3BD54-E633-4ED7-B627-6D1DEAD1E311}" name="ALAMAT SEBELUMNYA" dataDxfId="3" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{E462B6DD-29D4-4A17-AA0F-9EA81F6FD241}" name="TELEPON" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{470FBA59-E537-4ED4-BD1C-17FECE5E79A6}" name="EMAIL" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{861A2621-6363-4E65-B747-DE7EBE497051}" name="TANGGAL UPDATE DATA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6423,8 +6363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F398AC14-6103-402D-9DD1-504893389026}">
   <dimension ref="A1:AC501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B396" sqref="B396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43043,7 +42983,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>